<commit_message>
fixed protocol, minor protocol update
</commit_message>
<xml_diff>
--- a/Doc/protocol.xlsx
+++ b/Doc/protocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="140">
   <si>
     <t>0x11</t>
   </si>
@@ -302,9 +302,6 @@
     <t>save to EEPROM</t>
   </si>
   <si>
-    <t>U, I, brightness, temp</t>
-  </si>
-  <si>
     <t>&lt;Val&gt;</t>
   </si>
   <si>
@@ -432,6 +429,12 @@
   </si>
   <si>
     <t>Individual LED control</t>
+  </si>
+  <si>
+    <t>U, I, brightness, temp, fps</t>
+  </si>
+  <si>
+    <t>FPS: Frames/sec</t>
   </si>
 </sst>
 </file>
@@ -633,9 +636,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -643,6 +643,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -956,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +981,7 @@
         <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>81</v>
@@ -990,7 +993,7 @@
         <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -1000,7 +1003,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="G4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I4" t="s">
         <v>19</v>
@@ -1020,7 +1023,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -1037,7 +1040,7 @@
         <v>56</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
@@ -1050,6 +1053,9 @@
       <c r="C7" t="s">
         <v>32</v>
       </c>
+      <c r="G7" s="2" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1059,10 +1065,10 @@
         <v>33</v>
       </c>
       <c r="D8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>96</v>
       </c>
       <c r="F8" s="9"/>
       <c r="I8" s="1" t="s">
@@ -1144,7 +1150,7 @@
         <v>72</v>
       </c>
       <c r="I14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1165,10 +1171,10 @@
         <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1203,7 +1209,7 @@
         <v>63</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" t="s">
         <v>80</v>
@@ -1449,7 +1455,7 @@
         <v>63</v>
       </c>
       <c r="F30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="10:10" x14ac:dyDescent="0.25">
@@ -1465,7 +1471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -1479,28 +1485,28 @@
         <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
         <v>109</v>
-      </c>
-      <c r="C3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
         <v>111</v>
-      </c>
-      <c r="C4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
         <v>60</v>
@@ -1508,229 +1514,229 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s">
         <v>115</v>
-      </c>
-      <c r="C7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="13" t="s">
+      <c r="D9" s="19" t="s">
         <v>120</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="12" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17" t="s">
+      <c r="D11" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="19" t="s">
+      <c r="G11" s="16"/>
+      <c r="H11" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F12" t="s">
         <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>124</v>
-      </c>
-      <c r="H12" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>105</v>
+        <v>127</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F13" t="s">
         <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>124</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>117</v>
+        <v>123</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="19" t="s">
+      <c r="D14" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>104</v>
+        <v>129</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>103</v>
       </c>
       <c r="D15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G15" t="s">
-        <v>124</v>
-      </c>
-      <c r="H15" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="G16" t="s">
-        <v>124</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="19" t="s">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
-      </c>
-      <c r="H18" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C19" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>123</v>
-      </c>
-      <c r="H19" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>135</v>
-      </c>
-      <c r="C20" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
-      </c>
-      <c r="H20" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>119</v>
+        <v>135</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>118</v>
       </c>
       <c r="E21" t="s">
-        <v>123</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>118</v>
+        <v>122</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix, updated protocol_rev, changed cmd_test response
</commit_message>
<xml_diff>
--- a/Doc/protocol.xlsx
+++ b/Doc/protocol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="141">
   <si>
     <t>0x11</t>
   </si>
@@ -185,9 +185,6 @@
     <t>voltage</t>
   </si>
   <si>
-    <t>"LED", Status, Version</t>
-  </si>
-  <si>
     <t>LED:</t>
   </si>
   <si>
@@ -435,6 +432,12 @@
   </si>
   <si>
     <t>FPS: Frames/sec</t>
+  </si>
+  <si>
+    <t>"LED", Protocol_rev, SW_rev, HW_rev, Status</t>
+  </si>
+  <si>
+    <t>Protocol_rev</t>
   </si>
 </sst>
 </file>
@@ -960,7 +963,7 @@
   <dimension ref="A2:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,11 +983,14 @@
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -992,8 +998,11 @@
       <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -1003,7 +1012,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I4" t="s">
         <v>19</v>
@@ -1023,7 +1032,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -1037,10 +1046,10 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>139</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
@@ -1054,7 +1063,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1065,14 +1074,14 @@
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="9"/>
       <c r="I8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1083,7 +1092,7 @@
         <v>34</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1097,26 +1106,26 @@
         <v>45</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
         <v>92</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>93</v>
       </c>
-      <c r="D11" t="s">
-        <v>94</v>
-      </c>
       <c r="I11" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I12" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1130,7 +1139,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="I13" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1138,19 +1147,19 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1162,19 +1171,19 @@
         <v>-Default</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1186,13 +1195,13 @@
         <v>-Timeout</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1206,13 +1215,13 @@
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -1220,19 +1229,19 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -1247,38 +1256,38 @@
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" t="s">
         <v>85</v>
-      </c>
-      <c r="E20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
@@ -1287,47 +1296,47 @@
         <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
         <v>76</v>
       </c>
-      <c r="D23" t="s">
-        <v>77</v>
-      </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
@@ -1341,10 +1350,10 @@
         <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -1358,10 +1367,10 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1375,13 +1384,13 @@
         <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1395,13 +1404,13 @@
         <v>50</v>
       </c>
       <c r="E27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" t="s">
         <v>63</v>
       </c>
-      <c r="F27" t="s">
-        <v>64</v>
-      </c>
       <c r="G27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -1415,10 +1424,10 @@
         <v>52</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1432,13 +1441,13 @@
         <v>50</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
@@ -1452,10 +1461,10 @@
         <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="10:10" x14ac:dyDescent="0.25">
@@ -1485,64 +1494,64 @@
         <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
         <v>108</v>
-      </c>
-      <c r="C3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
         <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
         <v>114</v>
-      </c>
-      <c r="C7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1558,17 +1567,17 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="18" t="s">
@@ -1577,19 +1586,19 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>37</v>
@@ -1597,33 +1606,33 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -1634,16 +1643,16 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>37</v>
@@ -1651,16 +1660,16 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H16" s="13" t="s">
         <v>38</v>
@@ -1668,14 +1677,14 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -1685,13 +1694,13 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>37</v>
@@ -1699,13 +1708,13 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>38</v>
@@ -1713,13 +1722,13 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H20" s="13" t="s">
         <v>39</v>
@@ -1727,16 +1736,16 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dozens of small fixes and improvements, added brownout prevention, adc wip, usb and gamma done
</commit_message>
<xml_diff>
--- a/Doc/protocol.xlsx
+++ b/Doc/protocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="140">
   <si>
     <t>0x11</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Timeout.Time</t>
   </si>
   <si>
-    <t>Vbus / Time / Off</t>
-  </si>
-  <si>
     <t>Multi-LED</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>LEDs</t>
   </si>
   <si>
-    <t>"tLED"</t>
-  </si>
-  <si>
     <t>preamble</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t>values</t>
   </si>
   <si>
-    <t>(send twice)</t>
-  </si>
-  <si>
     <t>Stat-LED</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>0-20.4 A (80 mA)</t>
   </si>
   <si>
-    <t>0-255 pcs (1 pcs)</t>
-  </si>
-  <si>
     <t>0x00 - Off</t>
   </si>
   <si>
@@ -227,9 +215,6 @@
     <t>0-100 % (.39 %)</t>
   </si>
   <si>
-    <t>Limit: XMega64 - 80, Xmega128 - 160</t>
-  </si>
-  <si>
     <t>&lt;Mode&gt;</t>
   </si>
   <si>
@@ -254,9 +239,6 @@
     <t>0x00 - Auto</t>
   </si>
   <si>
-    <t>0x00 - Vbus detect, 0xFF - Off</t>
-  </si>
-  <si>
     <t>button:</t>
   </si>
   <si>
@@ -272,12 +254,6 @@
     <t>gamma value</t>
   </si>
   <si>
-    <t>Min: 0.05</t>
-  </si>
-  <si>
-    <t>0-12.75</t>
-  </si>
-  <si>
     <t>0-10200 Lux (40 Lux)</t>
   </si>
   <si>
@@ -296,15 +272,9 @@
     <t>settings -store</t>
   </si>
   <si>
-    <t>save to EEPROM</t>
-  </si>
-  <si>
     <t>&lt;Val&gt;</t>
   </si>
   <si>
-    <t>&lt;Mode&gt;+128 (MSB) -&gt; Standby - prev. Mode</t>
-  </si>
-  <si>
     <t>Menu</t>
   </si>
   <si>
@@ -332,9 +302,6 @@
     <t>Init</t>
   </si>
   <si>
-    <t>0-51 s (.2 s)</t>
-  </si>
-  <si>
     <t>0-5.1 V (20 mV)</t>
   </si>
   <si>
@@ -365,9 +332,6 @@
     <t>0x08</t>
   </si>
   <si>
-    <t>0x0F</t>
-  </si>
-  <si>
     <t>Other Err</t>
   </si>
   <si>
@@ -389,39 +353,6 @@
     <t>uid</t>
   </si>
   <si>
-    <t>0xA0</t>
-  </si>
-  <si>
-    <t>0xB1</t>
-  </si>
-  <si>
-    <t>0xB8</t>
-  </si>
-  <si>
-    <t>0x80</t>
-  </si>
-  <si>
-    <t>0x91</t>
-  </si>
-  <si>
-    <t>0x92</t>
-  </si>
-  <si>
-    <t>0x40</t>
-  </si>
-  <si>
-    <t>0x41</t>
-  </si>
-  <si>
-    <t>0x42</t>
-  </si>
-  <si>
-    <t>0x43</t>
-  </si>
-  <si>
-    <t>0x4F</t>
-  </si>
-  <si>
     <t>uint8</t>
   </si>
   <si>
@@ -438,6 +369,72 @@
   </si>
   <si>
     <t>Protocol_rev</t>
+  </si>
+  <si>
+    <t>"LeD"</t>
+  </si>
+  <si>
+    <t>0-25.5 s (.1 s)</t>
+  </si>
+  <si>
+    <t>Ack</t>
+  </si>
+  <si>
+    <t>Ack if write is done</t>
+  </si>
+  <si>
+    <t>(send adress twice, then data twice)</t>
+  </si>
+  <si>
+    <t>(store to EEPROM)</t>
+  </si>
+  <si>
+    <t>Min: 0.1</t>
+  </si>
+  <si>
+    <t>0-12.7</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>&lt;0x00, 0x01, 0x02, 0x03&gt;</t>
+  </si>
+  <si>
+    <t>(default_mode: set previous mode)</t>
+  </si>
+  <si>
+    <t>(bit 6: Set previous mode after standby)</t>
+  </si>
+  <si>
+    <t>oversample</t>
+  </si>
+  <si>
+    <t>oversample mode</t>
+  </si>
+  <si>
+    <t>&lt;Off, 2xMS, 4xMS, 8xMS&gt;</t>
+  </si>
+  <si>
+    <t>Vbus / Time</t>
+  </si>
+  <si>
+    <t>0x00 - Vbus detect only</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>0-160 pcs (1 pcs)</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>BOP</t>
+  </si>
+  <si>
+    <t>(hardcoded UVP of 4.0V to prevent brownout)</t>
   </si>
 </sst>
 </file>
@@ -528,7 +525,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -602,9 +599,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -612,21 +607,54 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -645,10 +673,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -960,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J42"/>
+  <dimension ref="A2:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,61 +1016,61 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
         <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1043,16 +1078,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1060,10 +1095,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1071,17 +1109,17 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F8" s="9"/>
       <c r="I8" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1089,57 +1127,66 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>135</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>121</v>
+      </c>
+      <c r="E10" t="s">
+        <v>122</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>120</v>
+      </c>
+      <c r="E11" t="s">
+        <v>123</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I12" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="I13" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1147,328 +1194,345 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" t="str">
         <f>"-Default"</f>
         <v>-Default</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G15" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" t="str">
         <f>"-Timeout"</f>
         <v>-Timeout</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="G17" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>0</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C20" t="str">
         <f>"-Default"</f>
         <v>-Default</v>
       </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="s">
-        <v>82</v>
-      </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>64</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
         <v>23</v>
       </c>
-      <c r="D25" t="s">
-        <v>24</v>
-      </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="G28" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F29" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" t="s">
         <v>62</v>
       </c>
-      <c r="F30" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J42" s="8"/>
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J43" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1478,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H21"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,266 +1555,306 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+        <v>34</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="12" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>7</v>
+      <c r="B11" s="21" t="str">
+        <f>IF(AND(D11="",E11="",F11="",G11=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H11,1))+IF(G11="Multi",16,0)+IF(F11="USB",32,0)+IF(E11="Err",64,0)+IF(D11="On",128,0))</f>
+        <v>0xA0</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>6</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G11" s="16"/>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>6</v>
+      <c r="B12" s="21" t="str">
+        <f t="shared" ref="B12:B22" si="0">IF(AND(D12="",E12="",F12="",G12=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H12,1))+IF(G12="Multi",16,0)+IF(F12="USB",32,0)+IF(E12="Err",64,0)+IF(D12="On",128,0))</f>
+        <v>0xB1</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>103</v>
+      <c r="B13" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0xB8</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>11</v>
+      <c r="B14" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x80</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="17" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>102</v>
+      <c r="B15" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x91</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G15" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>10</v>
+      <c r="B16" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0x92</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x40</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="17"/>
       <c r="E17" s="16" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>121</v>
-      </c>
+      <c r="I17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x41</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
       <c r="H18" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x42</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x43</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s">
-        <v>121</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="s">
-        <v>121</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>117</v>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x44</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>116</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x45</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new protocol doc (prevent merge problems)
</commit_message>
<xml_diff>
--- a/Doc/protocol.xlsx
+++ b/Doc/protocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="140">
   <si>
     <t>0x11</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Timeout.Time</t>
   </si>
   <si>
-    <t>Vbus / Time / Off</t>
-  </si>
-  <si>
     <t>Multi-LED</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>LEDs</t>
   </si>
   <si>
-    <t>"tLED"</t>
-  </si>
-  <si>
     <t>preamble</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t>values</t>
   </si>
   <si>
-    <t>(send twice)</t>
-  </si>
-  <si>
     <t>Stat-LED</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>0-20.4 A (80 mA)</t>
   </si>
   <si>
-    <t>0-255 pcs (1 pcs)</t>
-  </si>
-  <si>
     <t>0x00 - Off</t>
   </si>
   <si>
@@ -227,9 +215,6 @@
     <t>0-100 % (.39 %)</t>
   </si>
   <si>
-    <t>Limit: XMega64 - 80, Xmega128 - 160</t>
-  </si>
-  <si>
     <t>&lt;Mode&gt;</t>
   </si>
   <si>
@@ -254,9 +239,6 @@
     <t>0x00 - Auto</t>
   </si>
   <si>
-    <t>0x00 - Vbus detect, 0xFF - Off</t>
-  </si>
-  <si>
     <t>button:</t>
   </si>
   <si>
@@ -272,12 +254,6 @@
     <t>gamma value</t>
   </si>
   <si>
-    <t>Min: 0.05</t>
-  </si>
-  <si>
-    <t>0-12.75</t>
-  </si>
-  <si>
     <t>0-10200 Lux (40 Lux)</t>
   </si>
   <si>
@@ -296,15 +272,9 @@
     <t>settings -store</t>
   </si>
   <si>
-    <t>save to EEPROM</t>
-  </si>
-  <si>
     <t>&lt;Val&gt;</t>
   </si>
   <si>
-    <t>&lt;Mode&gt;+128 (MSB) -&gt; Standby - prev. Mode</t>
-  </si>
-  <si>
     <t>Menu</t>
   </si>
   <si>
@@ -332,9 +302,6 @@
     <t>Init</t>
   </si>
   <si>
-    <t>0-51 s (.2 s)</t>
-  </si>
-  <si>
     <t>0-5.1 V (20 mV)</t>
   </si>
   <si>
@@ -365,9 +332,6 @@
     <t>0x08</t>
   </si>
   <si>
-    <t>0x0F</t>
-  </si>
-  <si>
     <t>Other Err</t>
   </si>
   <si>
@@ -407,13 +371,70 @@
     <t>Protocol_rev</t>
   </si>
   <si>
-    <t>0xFF</t>
-  </si>
-  <si>
-    <t>reset</t>
-  </si>
-  <si>
-    <t>send 0xF0 0xF0 (application) or 0x0F 0x0F (bootloader)</t>
+    <t>"LeD"</t>
+  </si>
+  <si>
+    <t>0-25.5 s (.1 s)</t>
+  </si>
+  <si>
+    <t>Ack</t>
+  </si>
+  <si>
+    <t>Ack if write is done</t>
+  </si>
+  <si>
+    <t>(send adress twice, then data twice)</t>
+  </si>
+  <si>
+    <t>(store to EEPROM)</t>
+  </si>
+  <si>
+    <t>Min: 0.1</t>
+  </si>
+  <si>
+    <t>0-12.7</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>&lt;0x00, 0x01, 0x02, 0x03&gt;</t>
+  </si>
+  <si>
+    <t>(default_mode: set previous mode)</t>
+  </si>
+  <si>
+    <t>(bit 6: Set previous mode after standby)</t>
+  </si>
+  <si>
+    <t>oversample</t>
+  </si>
+  <si>
+    <t>oversample mode</t>
+  </si>
+  <si>
+    <t>&lt;Off, 2xMS, 4xMS, 8xMS&gt;</t>
+  </si>
+  <si>
+    <t>Vbus / Time</t>
+  </si>
+  <si>
+    <t>0x00 - Vbus detect only</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>0-160 pcs (1 pcs)</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>BOP</t>
+  </si>
+  <si>
+    <t>(hardcoded UVP of 4.0V to prevent brownout)</t>
   </si>
 </sst>
 </file>
@@ -590,9 +611,16 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -614,16 +642,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -633,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -655,6 +676,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -663,38 +688,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1003,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,61 +1016,61 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
         <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1084,16 +1078,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1101,10 +1095,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1112,17 +1109,17 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F8" s="9"/>
       <c r="I8" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1130,170 +1127,188 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>135</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>121</v>
+      </c>
+      <c r="E10" t="s">
+        <v>122</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>120</v>
+      </c>
+      <c r="E11" t="s">
+        <v>123</v>
       </c>
       <c r="I11" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="I13" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" t="s">
-        <v>132</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I13" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
       <c r="I14" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>89</v>
+        <v>35</v>
+      </c>
+      <c r="C15" t="str">
+        <f>"-Default"</f>
+        <v>-Default</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="G15" t="s">
+        <v>129</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="str">
-        <f>"-Default"</f>
-        <v>-Default</v>
+        <f>"-Timeout"</f>
+        <v>-Timeout</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="str">
-        <f>"-Timeout"</f>
-        <v>-Timeout</v>
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>119</v>
+      </c>
+      <c r="G17" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -1305,181 +1320,178 @@
         <v>-Default</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
         <v>13</v>
       </c>
-      <c r="D22" t="s">
-        <v>14</v>
-      </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
         <v>23</v>
       </c>
-      <c r="D26" t="s">
-        <v>24</v>
-      </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
         <v>26</v>
       </c>
-      <c r="D27" t="s">
-        <v>27</v>
-      </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F28" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" t="s">
         <v>63</v>
-      </c>
-      <c r="G28" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
@@ -1487,36 +1499,36 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" t="s">
         <v>62</v>
       </c>
-      <c r="F30" t="s">
-        <v>65</v>
-      </c>
       <c r="G30" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E31" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F31" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="10:10" x14ac:dyDescent="0.25">
@@ -1530,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H21"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,76 +1555,82 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
       <c r="H9" s="12" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="str">
-        <f>IF(AND(D10="",E10="",F10="",G10=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H10,1))+IF(G10="Multi",16,0)+IF(F10="USB",32,0)+IF(E10="Err",64,0)+IF(D10="On",128,0))</f>
-        <v>0x00</v>
+      <c r="B10" s="24" t="s">
+        <v>1</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>1</v>
@@ -1620,18 +1638,18 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="str">
-        <f t="shared" ref="B11:B21" si="0">IF(AND(D11="",E11="",F11="",G11=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H11,1))+IF(G11="Multi",16,0)+IF(F11="USB",32,0)+IF(E11="Err",64,0)+IF(D11="On",128,0))</f>
+        <f>IF(AND(D11="",E11="",F11="",G11=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H11,1))+IF(G11="Multi",16,0)+IF(F11="USB",32,0)+IF(E11="Err",64,0)+IF(D11="On",128,0))</f>
         <v>0xA0</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>7</v>
+      <c r="C11" s="23" t="s">
+        <v>6</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="17" t="s">
@@ -1640,23 +1658,23 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B12:B22" si="0">IF(AND(D12="",E12="",F12="",G12=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H12,1))+IF(G12="Multi",16,0)+IF(F12="USB",32,0)+IF(E12="Err",64,0)+IF(D12="On",128,0))</f>
         <v>0xB1</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1665,19 +1683,19 @@
         <v>0xB8</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1685,11 +1703,11 @@
         <f t="shared" si="0"/>
         <v>0x80</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>11</v>
+      <c r="C14" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -1704,16 +1722,16 @@
         <v>0x91</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G15" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1722,103 +1740,122 @@
         <v>0x92</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="str">
         <f t="shared" si="0"/>
         <v>0x40</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="16"/>
+      <c r="C17" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="17"/>
       <c r="E17" s="16" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="str">
         <f t="shared" si="0"/>
         <v>0x41</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>121</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
       <c r="H18" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="str">
         <f t="shared" si="0"/>
         <v>0x42</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="21" t="str">
         <f t="shared" si="0"/>
         <v>0x43</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>0x4F</v>
+        <v>0x44</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>116</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>0x45</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B10:B101">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
exported settings / sled, misc / adc functions -> set_sled, misc_adc lib
</commit_message>
<xml_diff>
--- a/Doc/protocol.xlsx
+++ b/Doc/protocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="138">
   <si>
     <t>0x11</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Stb-LED</t>
   </si>
   <si>
-    <t>Off / Alpha</t>
-  </si>
-  <si>
     <t>XL - Reset</t>
   </si>
   <si>
@@ -161,15 +158,6 @@
     <t>Off / Val</t>
   </si>
   <si>
-    <t>OCP.time</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>0x32</t>
-  </si>
-  <si>
     <t>0x34</t>
   </si>
   <si>
@@ -197,15 +185,6 @@
     <t>8 bit</t>
   </si>
   <si>
-    <t>0-10.2 A (40 mA)</t>
-  </si>
-  <si>
-    <t>0-255 ms (1 ms)</t>
-  </si>
-  <si>
-    <t>0-20.4 A (80 mA)</t>
-  </si>
-  <si>
     <t>0x00 - Off</t>
   </si>
   <si>
@@ -389,12 +368,6 @@
     <t>(store to EEPROM)</t>
   </si>
   <si>
-    <t>Min: 0.1</t>
-  </si>
-  <si>
-    <t>0-12.7</t>
-  </si>
-  <si>
     <t>0x04</t>
   </si>
   <si>
@@ -425,9 +398,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>0-160 pcs (1 pcs)</t>
-  </si>
-  <si>
     <t>0x05</t>
   </si>
   <si>
@@ -435,13 +405,37 @@
   </si>
   <si>
     <t>(hardcoded UVP of 4.0V to prevent brownout)</t>
+  </si>
+  <si>
+    <t>0-9.9</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>0-4.1 A (65 mA)</t>
+  </si>
+  <si>
+    <t>1-160 pcs (1 pcs)</t>
+  </si>
+  <si>
+    <t>Min: 1, Max: 160</t>
+  </si>
+  <si>
+    <t>Min: 1, Max: 99</t>
+  </si>
+  <si>
+    <t>0x00 - Off, Max: 63</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,6 +470,19 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -654,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -673,17 +680,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -995,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J43"/>
+  <dimension ref="A2:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,28 +1025,28 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -1047,7 +1056,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -1059,15 +1068,15 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
@@ -1078,16 +1087,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1095,13 +1104,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1109,17 +1118,17 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F8" s="9"/>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1127,13 +1136,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1141,52 +1150,54 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I12" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="23"/>
       <c r="I13" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1194,121 +1205,121 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="F14" t="s">
-        <v>66</v>
-      </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="str">
         <f>"-Default"</f>
         <v>-Default</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="F15" t="s">
-        <v>66</v>
-      </c>
       <c r="G15" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="str">
         <f>"-Timeout"</f>
         <v>-Timeout</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="26" t="s">
         <v>59</v>
-      </c>
-      <c r="F16" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" t="s">
-        <v>119</v>
+        <v>55</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="G17" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" t="s">
-        <v>127</v>
+        <v>55</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>118</v>
       </c>
       <c r="G18" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -1323,38 +1334,38 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" t="s">
-        <v>125</v>
+        <v>55</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>130</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -1363,176 +1374,162 @@
         <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" t="s">
-        <v>64</v>
+        <v>55</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="G22" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" t="s">
-        <v>80</v>
+        <v>55</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" t="s">
-        <v>79</v>
+        <v>55</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
         <v>25</v>
       </c>
-      <c r="D27" t="s">
-        <v>26</v>
-      </c>
       <c r="E27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" t="s">
-        <v>136</v>
+        <v>55</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>133</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="G29" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" t="s">
-        <v>59</v>
-      </c>
-      <c r="F31" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J43" s="8"/>
+        <v>55</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1544,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -1555,78 +1552,78 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+        <v>92</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+        <v>33</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="12" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -1637,19 +1634,19 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="str">
+      <c r="B11" s="19" t="str">
         <f>IF(AND(D11="",E11="",F11="",G11=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H11,1))+IF(G11="Multi",16,0)+IF(F11="USB",32,0)+IF(E11="Err",64,0)+IF(D11="On",128,0))</f>
         <v>0xA0</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="17" t="s">
@@ -1657,57 +1654,57 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="str">
+      <c r="B12" s="19" t="str">
         <f t="shared" ref="B12:B22" si="0">IF(AND(D12="",E12="",F12="",G12=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H12,1))+IF(G12="Multi",16,0)+IF(F12="USB",32,0)+IF(E12="Err",64,0)+IF(D12="On",128,0))</f>
         <v>0xB1</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="str">
+      <c r="B13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>0xB8</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>93</v>
+      <c r="C13" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="str">
+      <c r="B14" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x80</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="21" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -1717,52 +1714,52 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="str">
+      <c r="B15" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x91</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>92</v>
+      <c r="C15" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G15" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="str">
+      <c r="B16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>0x92</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G16" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="str">
+      <c r="B17" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x40</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>138</v>
+      <c r="C17" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="16" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -1770,85 +1767,85 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="str">
+      <c r="B18" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x41</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="str">
+      <c r="B19" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x42</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="19" t="s">
         <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="str">
+      <c r="B20" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x43</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="str">
+      <c r="B21" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x44</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="19" t="s">
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="str">
+      <c r="B22" s="19" t="str">
         <f t="shared" si="0"/>
         <v>0x45</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>105</v>
+      <c r="C22" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inplemented debug tools, reduced adc sample rate, added alpha control, added max value log, removed old error handling, rewrote sled control, fixed ada
</commit_message>
<xml_diff>
--- a/Doc/protocol.xlsx
+++ b/Doc/protocol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="119">
   <si>
     <t>0x11</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Photo-Delay</t>
   </si>
   <si>
-    <t>UVP</t>
-  </si>
-  <si>
     <t>K - Ein/Aus</t>
   </si>
   <si>
@@ -71,12 +68,6 @@
     <t>K - Toggle</t>
   </si>
   <si>
-    <t>L - Set / Val</t>
-  </si>
-  <si>
-    <t>SCP</t>
-  </si>
-  <si>
     <t>Stb-LED</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>0x03</t>
   </si>
   <si>
-    <t>0x10</t>
-  </si>
-  <si>
     <t>response</t>
   </si>
   <si>
@@ -137,12 +125,6 @@
     <t>Stat-LED</t>
   </si>
   <si>
-    <t>Off / Val</t>
-  </si>
-  <si>
-    <t>voltage</t>
-  </si>
-  <si>
     <t>LED:</t>
   </si>
   <si>
@@ -176,15 +158,9 @@
     <t>&lt;Mode&gt;</t>
   </si>
   <si>
-    <t>0x12</t>
-  </si>
-  <si>
     <t>Alpha-min</t>
   </si>
   <si>
-    <t>0x13</t>
-  </si>
-  <si>
     <t>Lux-max</t>
   </si>
   <si>
@@ -200,15 +176,9 @@
     <t>button:</t>
   </si>
   <si>
-    <t>0x14</t>
-  </si>
-  <si>
     <t>Gamma</t>
   </si>
   <si>
-    <t>0x15</t>
-  </si>
-  <si>
     <t>gamma value</t>
   </si>
   <si>
@@ -230,9 +200,6 @@
     <t>settings -store</t>
   </si>
   <si>
-    <t>&lt;Val&gt;</t>
-  </si>
-  <si>
     <t>Menu</t>
   </si>
   <si>
@@ -269,9 +236,6 @@
     <t>Bit 6</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
     <t>Bit 5</t>
   </si>
   <si>
@@ -284,9 +248,6 @@
     <t>0x08</t>
   </si>
   <si>
-    <t>Other Err</t>
-  </si>
-  <si>
     <t>designator</t>
   </si>
   <si>
@@ -296,9 +257,6 @@
     <t>On</t>
   </si>
   <si>
-    <t>Err</t>
-  </si>
-  <si>
     <t>Multi</t>
   </si>
   <si>
@@ -311,15 +269,9 @@
     <t>Individual LED control</t>
   </si>
   <si>
-    <t>U, I, brightness, temp, fps</t>
-  </si>
-  <si>
     <t>FPS: Frames/sec</t>
   </si>
   <si>
-    <t>"LED", Protocol_rev, SW_rev, HW_rev, Status</t>
-  </si>
-  <si>
     <t>Protocol_rev</t>
   </si>
   <si>
@@ -332,18 +284,9 @@
     <t>Ack</t>
   </si>
   <si>
-    <t>Ack if write is done</t>
-  </si>
-  <si>
-    <t>(send adress twice, then data twice)</t>
-  </si>
-  <si>
     <t>(store to EEPROM)</t>
   </si>
   <si>
-    <t>0x04</t>
-  </si>
-  <si>
     <t>&lt;0x00, 0x01, 0x02, 0x03&gt;</t>
   </si>
   <si>
@@ -368,18 +311,6 @@
     <t>0x00 - Vbus detect only</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>BOP</t>
-  </si>
-  <si>
-    <t>(hardcoded UVP of 4.0V to prevent brownout)</t>
-  </si>
-  <si>
-    <t>0-9.9</t>
-  </si>
-  <si>
     <t>range</t>
   </si>
   <si>
@@ -392,31 +323,55 @@
     <t>Min: 1, Max: 160</t>
   </si>
   <si>
-    <t>Min: 1, Max: 99</t>
-  </si>
-  <si>
-    <t>0x0F</t>
-  </si>
-  <si>
-    <t>0-4.1 A (50 mA)</t>
-  </si>
-  <si>
-    <t>0x00 - Off, Max: 82</t>
-  </si>
-  <si>
-    <t>4.0-6.55 V (10 mV)</t>
-  </si>
-  <si>
-    <t>0x05</t>
-  </si>
-  <si>
-    <t>0x06</t>
-  </si>
-  <si>
-    <t>0x07</t>
-  </si>
-  <si>
-    <t>0x09</t>
+    <t>Ack, "LED", Protocol_rev, SW_rev, HW_rev, Status</t>
+  </si>
+  <si>
+    <t>Ack, U, I, brightness, temp, fps, U_min, I_max</t>
+  </si>
+  <si>
+    <t>Ack if ready for data</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>&lt;data after ack&gt;</t>
+  </si>
+  <si>
+    <t>&lt;address&gt;</t>
+  </si>
+  <si>
+    <t>&lt;address, value&gt;</t>
+  </si>
+  <si>
+    <t>Ack, address, value</t>
+  </si>
+  <si>
+    <t>read ALL</t>
+  </si>
+  <si>
+    <t>returns all set values, beginning with mode</t>
+  </si>
+  <si>
+    <t>Set if current mode = usb</t>
+  </si>
+  <si>
+    <t>0-25.5</t>
+  </si>
+  <si>
+    <t>L - Set</t>
+  </si>
+  <si>
+    <t>0x00 - Off (disables alpha and oversampling)</t>
+  </si>
+  <si>
+    <t>Caution: modes are not validated</t>
+  </si>
+  <si>
+    <t>reserved</t>
   </si>
 </sst>
 </file>
@@ -464,12 +419,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -520,7 +475,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -623,11 +578,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -647,23 +622,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -970,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J42"/>
+  <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,507 +970,510 @@
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
-    <col min="11" max="14" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="12" max="15" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+      <c r="H5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>71</v>
+        <v>106</v>
+      </c>
+      <c r="E8" t="s">
+        <v>103</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="I8" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G8" s="9"/>
+      <c r="J8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
         <v>106</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
       <c r="E11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="I13" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15">
         <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>32</v>
       </c>
       <c r="C15" t="str">
         <f>"-Default"</f>
         <v>-Default</v>
       </c>
-      <c r="D15" t="s">
-        <v>52</v>
-      </c>
       <c r="E15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" t="s">
-        <v>111</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
       </c>
       <c r="C16" t="str">
         <f>"-Timeout"</f>
         <v>-Timeout</v>
       </c>
-      <c r="D16" t="s">
-        <v>52</v>
-      </c>
       <c r="E16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
-        <v>115</v>
-      </c>
       <c r="E17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>108</v>
+        <v>96</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D18" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>130</v>
+        <v>94</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
         <v>11</v>
       </c>
-      <c r="E19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" t="s">
         <v>51</v>
       </c>
-      <c r="G19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>131</v>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>6</v>
       </c>
       <c r="C20" t="str">
         <f>"-Default"</f>
         <v>-Default</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>11</v>
       </c>
-      <c r="E20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" t="s">
         <v>51</v>
       </c>
-      <c r="G20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>132</v>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="G21" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>88</v>
+        <v>54</v>
+      </c>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>8</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>13</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="E24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="F24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
         <v>35</v>
       </c>
-      <c r="C24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" t="s">
-        <v>122</v>
-      </c>
       <c r="E25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>53</v>
+        <v>99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>12</v>
       </c>
       <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
         <v>20</v>
       </c>
-      <c r="D26" t="s">
-        <v>122</v>
-      </c>
-      <c r="E26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="G27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="G29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F30" s="19"/>
-    </row>
-    <row r="42" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J42" s="8"/>
+      <c r="F27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>255</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="18"/>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1491,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I22"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,88 +1496,88 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+        <v>118</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="22" t="s">
-        <v>90</v>
+      <c r="B9" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="21" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1598,11 +1590,11 @@
         <v>6</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="11" t="s">
@@ -1618,16 +1610,16 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1636,19 +1628,19 @@
         <v>0xB8</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
         <v>79</v>
       </c>
-      <c r="D13" t="s">
-        <v>92</v>
-      </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1660,7 +1652,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -1675,16 +1667,16 @@
         <v>0x91</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1692,89 +1684,49 @@
         <f t="shared" si="0"/>
         <v>0x92</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" t="s">
-        <v>94</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>0x40</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>0x41</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="str">
-        <f>IF(AND(D19="",E19="",F19="",G19=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H19,1))+IF(G19="Multi",16,0)+IF(F19="USB",32,0)+IF(E19="Err",64,0)+IF(D19="On",128,0))</f>
-        <v>0x42</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" t="s">
-        <v>93</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="15" t="str">
-        <f>IF(AND(D20="",E20="",F20="",G20=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H20,1))+IF(G20="Multi",16,0)+IF(F20="USB",32,0)+IF(E20="Err",64,0)+IF(D20="On",128,0))</f>
-        <v>0x4F</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
@@ -1788,6 +1740,10 @@
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="D4:H4"/>
   </mergeCells>
+  <conditionalFormatting sqref="B10:B25">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed IR, added new single-color-mode, corrected doc
</commit_message>
<xml_diff>
--- a/Doc/protocol.xlsx
+++ b/Doc/protocol.xlsx
@@ -1,34 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="1" r:id="rId1"/>
     <sheet name="Mode" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="119">
-  <si>
-    <t>0x11</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
   <si>
     <t>0x00</t>
   </si>
   <si>
-    <t>0x22</t>
-  </si>
-  <si>
-    <t>0x33</t>
-  </si>
-  <si>
     <t>Timeout.Time</t>
   </si>
   <si>
@@ -41,9 +32,6 @@
     <t>OFF</t>
   </si>
   <si>
-    <t>0x44</t>
-  </si>
-  <si>
     <t>Colorswirl</t>
   </si>
   <si>
@@ -192,9 +180,6 @@
   </si>
   <si>
     <t>Alpha (RAM)</t>
-  </si>
-  <si>
-    <t>0x55</t>
   </si>
   <si>
     <t>settings -store</t>
@@ -627,16 +612,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -961,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,197 +966,197 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>1</v>
+      <c r="B6">
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
         <v>102</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>107</v>
-      </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>2</v>
+      <c r="B8">
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="J8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>3</v>
+      <c r="B9">
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>8</v>
+      <c r="B10">
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>59</v>
+      <c r="B11">
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J12" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>117</v>
+        <v>93</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>112</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1179,19 +1164,19 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="18" t="s">
-        <v>46</v>
-      </c>
       <c r="J14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1203,19 +1188,19 @@
         <v>-Default</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="18" t="s">
-        <v>46</v>
-      </c>
       <c r="H15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1227,16 +1212,16 @@
         <v>-Timeout</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="18" t="s">
-        <v>46</v>
-      </c>
       <c r="H16" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1244,19 +1229,19 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H17" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1264,19 +1249,19 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G18" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" t="s">
         <v>90</v>
-      </c>
-      <c r="H18" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1284,19 +1269,19 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1308,16 +1293,16 @@
         <v>-Default</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1325,19 +1310,19 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H21" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1345,19 +1330,19 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1365,16 +1350,16 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1382,16 +1367,16 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1399,16 +1384,16 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1416,16 +1401,16 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1433,19 +1418,19 @@
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H27" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1453,13 +1438,13 @@
         <v>255</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G28" s="18"/>
     </row>
@@ -1485,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,89 +1481,89 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+        <v>113</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+        <v>24</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
-        <v>1</v>
+      <c r="B10" s="26" t="s">
+        <v>0</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
       <c r="H10" s="23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -1587,39 +1572,39 @@
         <v>0xA0</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="str">
-        <f t="shared" ref="B12:B18" si="0">IF(AND(D12="",E12="",F12="",G12=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H12,1))+IF(G12="Multi",16,0)+IF(F12="USB",32,0)+IF(E12="Err",64,0)+IF(D12="On",128,0))</f>
+        <f t="shared" ref="B12:B16" si="0">IF(AND(D12="",E12="",F12="",G12=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H12,1))+IF(G12="Multi",16,0)+IF(F12="USB",32,0)+IF(E12="Err",64,0)+IF(D12="On",128,0))</f>
         <v>0xB1</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1628,19 +1613,19 @@
         <v>0xB8</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1649,16 +1634,16 @@
         <v>0x80</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -1667,16 +1652,16 @@
         <v>0x91</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1685,18 +1670,18 @@
         <v>0x92</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
-(Bugfix) USB Raw mode -Gamma .05 settings resolution -Variable FPS Limit -(Bugfix) Light measurement (x1/2 gain seems to add a big negative offset, hw-bug?)
</commit_message>
<xml_diff>
--- a/Doc/protocol.xlsx
+++ b/Doc/protocol.xlsx
@@ -8,36 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Cmd" sheetId="1" r:id="rId1"/>
-    <sheet name="Mode" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
-  <si>
-    <t>0x00</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
   <si>
     <t>Timeout.Time</t>
   </si>
   <si>
-    <t>Multi-LED</t>
-  </si>
-  <si>
-    <t>Single-LED</t>
-  </si>
-  <si>
-    <t>OFF</t>
-  </si>
-  <si>
-    <t>Colorswirl</t>
-  </si>
-  <si>
-    <t>Moodlamp</t>
-  </si>
-  <si>
     <t>Auto / Manual</t>
   </si>
   <si>
@@ -89,15 +70,6 @@
     <t>settings - set</t>
   </si>
   <si>
-    <t>mode</t>
-  </si>
-  <si>
-    <t>0x01</t>
-  </si>
-  <si>
-    <t>0x02</t>
-  </si>
-  <si>
     <t>0x03</t>
   </si>
   <si>
@@ -203,57 +175,9 @@
     <t>Temp: 1/10 °C</t>
   </si>
   <si>
-    <t>Rainbow</t>
-  </si>
-  <si>
-    <t>Adalight</t>
-  </si>
-  <si>
     <t>Init</t>
   </si>
   <si>
-    <t>Bit 7 (MSB)</t>
-  </si>
-  <si>
-    <t>LED On</t>
-  </si>
-  <si>
-    <t>Bit 6</t>
-  </si>
-  <si>
-    <t>Bit 5</t>
-  </si>
-  <si>
-    <t>Bit 4</t>
-  </si>
-  <si>
-    <t>Bit 3-0 (LSB)</t>
-  </si>
-  <si>
-    <t>0x08</t>
-  </si>
-  <si>
-    <t>designator</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>On</t>
-  </si>
-  <si>
-    <t>Multi</t>
-  </si>
-  <si>
-    <t>uid</t>
-  </si>
-  <si>
-    <t>uint8</t>
-  </si>
-  <si>
-    <t>Individual LED control</t>
-  </si>
-  <si>
     <t>FPS: Frames/sec</t>
   </si>
   <si>
@@ -275,9 +199,6 @@
     <t>&lt;0x00, 0x01, 0x02, 0x03&gt;</t>
   </si>
   <si>
-    <t>(default_mode: set previous mode)</t>
-  </si>
-  <si>
     <t>(bit 6: Set previous mode after standby)</t>
   </si>
   <si>
@@ -356,17 +277,47 @@
     <t>Caution: modes are not validated</t>
   </si>
   <si>
-    <t>reserved</t>
-  </si>
-  <si>
-    <t>data as little endian (LSB first)</t>
+    <t>Higher count requires &gt;4k SRAM</t>
+  </si>
+  <si>
+    <t>High count and oversample can lead to flickering at high update rates</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>set_sled:</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>define setting</t>
+  </si>
+  <si>
+    <t>Protocol:</t>
+  </si>
+  <si>
+    <t>default value (read_settings)</t>
+  </si>
+  <si>
+    <t>enum vars</t>
+  </si>
+  <si>
+    <t>init routine (read_settings)</t>
+  </si>
+  <si>
+    <t>create write routine</t>
+  </si>
+  <si>
+    <t>add write var (write_set)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +369,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -463,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -471,126 +429,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -602,55 +445,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -959,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,64 +782,64 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="J3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1044,19 +847,19 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1064,16 +867,16 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1081,21 +884,19 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="29" t="s">
-        <v>114</v>
-      </c>
+      <c r="H8" s="13"/>
       <c r="J8" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1103,16 +904,16 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1120,16 +921,16 @@
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1137,42 +938,42 @@
         <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J12" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>112</v>
+        <v>67</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1180,19 +981,19 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>42</v>
+        <v>29</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1204,19 +1005,19 @@
         <v>-Default</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>42</v>
+        <v>29</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1228,16 +1029,16 @@
         <v>-Timeout</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>42</v>
+        <v>29</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="H16" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1245,19 +1046,19 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>82</v>
+        <v>29</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="H17" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1265,19 +1066,19 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>85</v>
+        <v>29</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="H18" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1285,19 +1086,19 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" t="s">
         <v>38</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1309,16 +1110,16 @@
         <v>-Default</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
         <v>38</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1326,19 +1127,19 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>109</v>
+        <v>29</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1346,19 +1147,19 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="H22" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1366,16 +1167,16 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="E23" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1383,16 +1184,16 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>51</v>
+        <v>29</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1400,16 +1201,16 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>41</v>
+        <v>29</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1417,16 +1218,16 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="F26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>41</v>
+        <v>29</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1434,19 +1235,19 @@
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>95</v>
+        <v>29</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="H27" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1454,298 +1255,86 @@
         <v>255</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="18"/>
+        <v>81</v>
+      </c>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G29" s="18"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G30" s="18"/>
+      <c r="E30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="11"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G31" s="18"/>
-    </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E36" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E38" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E40" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E41" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K43" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H22"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="7" width="5.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="str">
-        <f>IF(AND(D10="",E10="",F10="",G10=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H10,1))+IF(G10="Multi",16,0)+IF(F10="USB",32,0)+IF(E10="Err",64,0)+IF(D10="On",128,0))</f>
-        <v>0x00</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="str">
-        <f>IF(AND(D11="",E11="",F11="",G11=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H11,1))+IF(G11="Multi",16,0)+IF(F11="USB",32,0)+IF(E11="Err",64,0)+IF(D11="On",128,0))</f>
-        <v>0xA0</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="str">
-        <f t="shared" ref="B12:B18" si="0">IF(AND(D12="",E12="",F12="",G12=""),"0x0","0x")&amp;DEC2HEX(HEX2DEC(RIGHT(H12,1))+IF(G12="Multi",16,0)+IF(F12="USB",32,0)+IF(E12="Err",64,0)+IF(D12="On",128,0))</f>
-        <v>0xB1</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>0xB8</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>0x80</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>0x91</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>0x92</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D4:H4"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B10:B25">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>